<commit_message>
update-uri la limitele de incredere
</commit_message>
<xml_diff>
--- a/statistici.xlsx
+++ b/statistici.xlsx
@@ -5,11 +5,11 @@
     <x:workbookView/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Date initiale" sheetId="1" r:id="R22252c9a1ee84ee2"/>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Validare" sheetId="2" r:id="R612e4c9397a64ad8"/>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Valori de interes" sheetId="3" r:id="R19001aa75856427c"/>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Preturi de referinta" sheetId="4" r:id="Rd9f20578da7849dd"/>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Rezultate economice" sheetId="5" r:id="R03d00fcdf9ef4b95"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Date initiale" sheetId="1" r:id="R34f355cf742749b2"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Validare" sheetId="2" r:id="R0a689c7415444918"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Valori de interes" sheetId="3" r:id="R788ebae74f0446cb"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Preturi de referinta" sheetId="4" r:id="Ra81668df37444421"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Rezultate economice" sheetId="5" r:id="R8712bf2afab345be"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -114,6 +114,24 @@
       <x:c r="G1" t="str">
         <x:v>f 5%</x:v>
       </x:c>
+      <x:c r="H1" t="str">
+        <x:v>Abatere</x:v>
+      </x:c>
+      <x:c r="I1" t="str">
+        <x:v>tp 80%</x:v>
+      </x:c>
+      <x:c r="J1" t="str">
+        <x:v>tp 90%</x:v>
+      </x:c>
+      <x:c r="K1" t="str">
+        <x:v>tp 95%</x:v>
+      </x:c>
+      <x:c r="L1" t="str">
+        <x:v>tp 99%</x:v>
+      </x:c>
+      <x:c r="M1" t="str">
+        <x:v>tp 99.9%</x:v>
+      </x:c>
     </x:row>
     <x:row r="2">
       <x:c r="A2" t="str">
@@ -132,10 +150,28 @@
         <x:v>0.9955911818611</x:v>
       </x:c>
       <x:c r="F2" t="str">
-        <x:v>10.92</x:v>
+        <x:v>13.27</x:v>
       </x:c>
       <x:c r="G2" t="str">
-        <x:v>5.14</x:v>
+        <x:v>5.79</x:v>
+      </x:c>
+      <x:c r="H2" t="str">
+        <x:v>304.613058889895</x:v>
+      </x:c>
+      <x:c r="I2" t="str">
+        <x:v>1.44</x:v>
+      </x:c>
+      <x:c r="J2" t="str">
+        <x:v>1.943</x:v>
+      </x:c>
+      <x:c r="K2" t="str">
+        <x:v>2.447</x:v>
+      </x:c>
+      <x:c r="L2" t="str">
+        <x:v>3.707</x:v>
+      </x:c>
+      <x:c r="M2" t="str">
+        <x:v>5.959</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>